<commit_message>
Added student profile page with photo and marksheet display
</commit_message>
<xml_diff>
--- a/masterstudent.xlsx
+++ b/masterstudent.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\DJANGO_GPT\visitor_mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="226">
   <si>
     <t>DOB</t>
   </si>
@@ -664,13 +664,46 @@
   </si>
   <si>
     <t>student_class</t>
+  </si>
+  <si>
+    <t>Bhavani</t>
+  </si>
+  <si>
+    <t>bcom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhavani </t>
+  </si>
+  <si>
+    <t>Gohil</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>chokdi</t>
+  </si>
+  <si>
+    <t>XXXXXXXX3584</t>
+  </si>
+  <si>
+    <t>bhavanising008@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>photos/2021-013.jpg</t>
+  </si>
+  <si>
+    <t>2021-013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +715,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -719,16 +760,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1031,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1961,51 @@
         <v>203</v>
       </c>
     </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F22" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" t="s">
+        <v>220</v>
+      </c>
+      <c r="H22">
+        <v>8347078272</v>
+      </c>
+      <c r="I22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K22" t="s">
+        <v>223</v>
+      </c>
+      <c r="L22" s="3">
+        <v>39646</v>
+      </c>
+      <c r="M22" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J22" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated student documents + notice system + improvements in student proofile like change pass forgot pass via email or mobile.
</commit_message>
<xml_diff>
--- a/masterstudent.xlsx
+++ b/masterstudent.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="243">
   <si>
     <t>DOB</t>
   </si>
@@ -697,6 +697,57 @@
   </si>
   <si>
     <t>2021-013</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>yash</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>prajapati</t>
+  </si>
+  <si>
+    <t>bholad</t>
+  </si>
+  <si>
+    <t>yash@gmail.com</t>
+  </si>
+  <si>
+    <t>photos/2029-008.jpg</t>
+  </si>
+  <si>
+    <t>2019-008</t>
+  </si>
+  <si>
+    <t>2022-037</t>
+  </si>
+  <si>
+    <t>Mukesh</t>
+  </si>
+  <si>
+    <t>Mahadevbhai</t>
+  </si>
+  <si>
+    <t>kolipatel</t>
+  </si>
+  <si>
+    <t>Kamijala</t>
+  </si>
+  <si>
+    <t>mukesh@gmail.com</t>
+  </si>
+  <si>
+    <t>photos/2022-037.jpg</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1147,8 @@
     <col min="10" max="10" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1139,7 +1191,9 @@
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2002,9 +2056,87 @@
         <v>224</v>
       </c>
     </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" t="s">
+        <v>230</v>
+      </c>
+      <c r="F23" t="s">
+        <v>231</v>
+      </c>
+      <c r="G23" t="s">
+        <v>232</v>
+      </c>
+      <c r="H23">
+        <v>9638845196</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K23" t="s">
+        <v>163</v>
+      </c>
+      <c r="L23" s="3">
+        <v>38818</v>
+      </c>
+      <c r="M23" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>237</v>
+      </c>
+      <c r="E24" t="s">
+        <v>238</v>
+      </c>
+      <c r="F24" t="s">
+        <v>239</v>
+      </c>
+      <c r="G24" t="s">
+        <v>240</v>
+      </c>
+      <c r="H24">
+        <v>8347898768</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K24" t="s">
+        <v>223</v>
+      </c>
+      <c r="L24" s="3">
+        <v>39927</v>
+      </c>
+      <c r="M24" t="s">
+        <v>242</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J22" r:id="rId1"/>
+    <hyperlink ref="J23" r:id="rId2"/>
+    <hyperlink ref="J24" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Created a full face attendence system with csv file When we scan face then our attendence marked as P in attendence.csv file. this is 95% accurate
</commit_message>
<xml_diff>
--- a/masterstudent.xlsx
+++ b/masterstudent.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="252">
   <si>
     <t>DOB</t>
   </si>
@@ -748,6 +749,33 @@
   </si>
   <si>
     <t>photos/2022-037.jpg</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mon  </t>
+  </si>
+  <si>
+    <t>tue</t>
+  </si>
+  <si>
+    <t>wed</t>
+  </si>
+  <si>
+    <t>thue</t>
+  </si>
+  <si>
+    <t>fri</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -2140,4 +2168,544 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
+      </c>
+      <c r="P2">
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <v>13</v>
+      </c>
+      <c r="R2">
+        <v>14</v>
+      </c>
+      <c r="S2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H3" t="s">
+        <v>246</v>
+      </c>
+      <c r="I3" t="s">
+        <v>247</v>
+      </c>
+      <c r="J3" t="s">
+        <v>248</v>
+      </c>
+      <c r="K3" t="s">
+        <v>249</v>
+      </c>
+      <c r="L3" t="s">
+        <v>243</v>
+      </c>
+      <c r="M3" t="s">
+        <v>244</v>
+      </c>
+      <c r="N3" t="s">
+        <v>245</v>
+      </c>
+      <c r="O3" t="s">
+        <v>246</v>
+      </c>
+      <c r="P3" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>248</v>
+      </c>
+      <c r="R3" t="s">
+        <v>249</v>
+      </c>
+      <c r="S3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" t="s">
+        <v>250</v>
+      </c>
+      <c r="K5" t="s">
+        <v>250</v>
+      </c>
+      <c r="L5" t="s">
+        <v>250</v>
+      </c>
+      <c r="M5" t="s">
+        <v>250</v>
+      </c>
+      <c r="N5" t="s">
+        <v>250</v>
+      </c>
+      <c r="O5" t="s">
+        <v>250</v>
+      </c>
+      <c r="P5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>250</v>
+      </c>
+      <c r="R5" t="s">
+        <v>250</v>
+      </c>
+      <c r="S5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G6" t="s">
+        <v>251</v>
+      </c>
+      <c r="H6" t="s">
+        <v>251</v>
+      </c>
+      <c r="I6" t="s">
+        <v>251</v>
+      </c>
+      <c r="J6" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" t="s">
+        <v>251</v>
+      </c>
+      <c r="L6" t="s">
+        <v>251</v>
+      </c>
+      <c r="M6" t="s">
+        <v>251</v>
+      </c>
+      <c r="N6" t="s">
+        <v>251</v>
+      </c>
+      <c r="O6" t="s">
+        <v>251</v>
+      </c>
+      <c r="P6" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>251</v>
+      </c>
+      <c r="R6" t="s">
+        <v>251</v>
+      </c>
+      <c r="S6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" t="s">
+        <v>229</v>
+      </c>
+      <c r="C26" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>